<commit_message>
translate all table xls in xlsx and delete unnecessary columns
</commit_message>
<xml_diff>
--- a/ai-2019_version-2.0/2018.xlsx
+++ b/ai-2019_version-2.0/2018.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexander/git/conference/ai-2019/version-2.0/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE45A4DD-EF25-9A45-A65B-A68D89D0870C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -1210,8 +1204,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1270,25 +1264,17 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1326,9 +1312,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1360,27 +1346,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1412,27 +1380,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1605,20 +1555,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H357"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A316" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="6" max="6" width="30.83203125" customWidth="1"/>
-    <col min="7" max="7" width="22.1640625" customWidth="1"/>
-    <col min="8" max="8" width="19.83203125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1641,7 +1585,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1667,7 +1611,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1693,7 +1637,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1719,7 +1663,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1745,7 +1689,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1771,7 +1715,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1797,7 +1741,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1823,7 +1767,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1849,7 +1793,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1875,7 +1819,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1883,7 +1827,7 @@
         <v>16</v>
       </c>
       <c r="C11">
-        <v>-19.899999999999999</v>
+        <v>-19.9</v>
       </c>
       <c r="D11">
         <v>750.3</v>
@@ -1901,7 +1845,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1927,7 +1871,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1953,7 +1897,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1979,7 +1923,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2005,7 +1949,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2031,7 +1975,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2057,7 +2001,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -2083,7 +2027,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -2091,7 +2035,7 @@
         <v>24</v>
       </c>
       <c r="C19">
-        <v>-8.1999999999999993</v>
+        <v>-8.199999999999999</v>
       </c>
       <c r="D19">
         <v>746</v>
@@ -2109,7 +2053,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2135,7 +2079,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2161,7 +2105,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2187,7 +2131,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -2213,7 +2157,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -2239,7 +2183,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -2247,7 +2191,7 @@
         <v>30</v>
       </c>
       <c r="C25">
-        <v>-18.100000000000001</v>
+        <v>-18.1</v>
       </c>
       <c r="D25">
         <v>753.4</v>
@@ -2265,7 +2209,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -2291,7 +2235,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2317,7 +2261,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -2343,7 +2287,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -2369,7 +2313,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -2395,7 +2339,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -2421,7 +2365,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -2447,7 +2391,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -2473,7 +2417,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -2499,7 +2443,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -2525,7 +2469,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -2551,7 +2495,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -2577,7 +2521,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -2603,7 +2547,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -2611,7 +2555,7 @@
         <v>44</v>
       </c>
       <c r="C39">
-        <v>-1.1000000000000001</v>
+        <v>-1.1</v>
       </c>
       <c r="D39">
         <v>732.2</v>
@@ -2629,7 +2573,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -2655,7 +2599,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -2681,7 +2625,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -2707,7 +2651,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -2733,7 +2677,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -2759,7 +2703,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -2785,7 +2729,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -2811,7 +2755,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -2837,7 +2781,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -2863,7 +2807,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -2889,7 +2833,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -2915,7 +2859,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -2941,7 +2885,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -2967,7 +2911,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -2975,7 +2919,7 @@
         <v>58</v>
       </c>
       <c r="C53">
-        <v>-1.1000000000000001</v>
+        <v>-1.1</v>
       </c>
       <c r="D53">
         <v>730.9</v>
@@ -2993,7 +2937,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -3019,7 +2963,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -3045,7 +2989,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -3071,7 +3015,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -3097,7 +3041,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -3123,7 +3067,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -3149,7 +3093,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -3175,7 +3119,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -3201,7 +3145,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -3227,7 +3171,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -3253,7 +3197,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -3279,7 +3223,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -3305,7 +3249,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -3331,7 +3275,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -3357,7 +3301,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -3383,7 +3327,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -3409,7 +3353,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -3435,7 +3379,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -3461,7 +3405,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -3469,7 +3413,7 @@
         <v>77</v>
       </c>
       <c r="C72">
-        <v>5.0999999999999996</v>
+        <v>5.1</v>
       </c>
       <c r="D72">
         <v>739</v>
@@ -3487,7 +3431,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -3513,7 +3457,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -3539,7 +3483,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -3565,7 +3509,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -3591,7 +3535,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -3617,7 +3561,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -3625,7 +3569,7 @@
         <v>83</v>
       </c>
       <c r="C78">
-        <v>16.100000000000001</v>
+        <v>16.1</v>
       </c>
       <c r="D78">
         <v>729.1</v>
@@ -3643,7 +3587,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -3669,7 +3613,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -3677,7 +3621,7 @@
         <v>85</v>
       </c>
       <c r="C80">
-        <v>4.0999999999999996</v>
+        <v>4.1</v>
       </c>
       <c r="D80">
         <v>744.1</v>
@@ -3695,7 +3639,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -3703,7 +3647,7 @@
         <v>86</v>
       </c>
       <c r="C81">
-        <v>9.1999999999999993</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="D81">
         <v>738.2</v>
@@ -3721,7 +3665,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -3747,7 +3691,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -3755,7 +3699,7 @@
         <v>88</v>
       </c>
       <c r="C83">
-        <v>8.8000000000000007</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="D83">
         <v>746.2</v>
@@ -3773,7 +3717,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -3799,7 +3743,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -3825,7 +3769,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -3851,7 +3795,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -3877,7 +3821,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -3903,7 +3847,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -3929,7 +3873,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -3955,7 +3899,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -3981,7 +3925,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -4007,7 +3951,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -4033,7 +3977,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -4059,7 +4003,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -4085,7 +4029,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -4093,7 +4037,7 @@
         <v>101</v>
       </c>
       <c r="C96">
-        <v>10.199999999999999</v>
+        <v>10.2</v>
       </c>
       <c r="D96">
         <v>740.9</v>
@@ -4111,7 +4055,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -4137,7 +4081,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -4163,7 +4107,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -4189,7 +4133,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -4215,7 +4159,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -4223,7 +4167,7 @@
         <v>106</v>
       </c>
       <c r="C101">
-        <v>16.399999999999999</v>
+        <v>16.4</v>
       </c>
       <c r="D101">
         <v>743.2</v>
@@ -4241,7 +4185,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:8">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -4267,7 +4211,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:8">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -4293,7 +4237,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:8">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -4319,7 +4263,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:8">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -4345,7 +4289,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:8">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -4371,7 +4315,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:8">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -4397,7 +4341,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:8">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -4423,7 +4367,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:8">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -4449,7 +4393,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:8">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -4475,7 +4419,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:8">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -4483,7 +4427,7 @@
         <v>116</v>
       </c>
       <c r="C111">
-        <v>19.899999999999999</v>
+        <v>19.9</v>
       </c>
       <c r="D111">
         <v>734.2</v>
@@ -4501,7 +4445,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:8">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -4527,7 +4471,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:8">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -4553,7 +4497,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:8">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -4579,7 +4523,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:8">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -4605,7 +4549,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:8">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -4613,7 +4557,7 @@
         <v>121</v>
       </c>
       <c r="C116">
-        <v>8.1999999999999993</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="D116">
         <v>741.4</v>
@@ -4631,7 +4575,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:8">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -4657,7 +4601,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:8">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -4683,7 +4627,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:8">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -4709,7 +4653,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:8">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -4735,7 +4679,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:8">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -4761,7 +4705,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:8">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -4787,7 +4731,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:8">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -4813,7 +4757,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:8">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -4821,7 +4765,7 @@
         <v>129</v>
       </c>
       <c r="C124">
-        <v>20.100000000000001</v>
+        <v>20.1</v>
       </c>
       <c r="D124">
         <v>732.3</v>
@@ -4839,7 +4783,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:8">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -4865,7 +4809,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:8">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -4891,7 +4835,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:8">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -4917,7 +4861,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:8">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -4943,7 +4887,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:8">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -4969,7 +4913,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:8">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -4995,7 +4939,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:8">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -5021,7 +4965,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:8">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -5047,7 +4991,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:8">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -5073,7 +5017,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:8">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -5099,7 +5043,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:8">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -5107,7 +5051,7 @@
         <v>140</v>
       </c>
       <c r="C135">
-        <v>19.399999999999999</v>
+        <v>19.4</v>
       </c>
       <c r="D135">
         <v>743</v>
@@ -5125,7 +5069,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:8">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -5151,7 +5095,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:8">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -5177,7 +5121,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:8">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -5203,7 +5147,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:8">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -5229,7 +5173,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:8">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -5255,7 +5199,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:8">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -5281,7 +5225,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:8">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -5307,7 +5251,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:8">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -5315,7 +5259,7 @@
         <v>148</v>
       </c>
       <c r="C143">
-        <v>17.899999999999999</v>
+        <v>17.9</v>
       </c>
       <c r="D143">
         <v>737.5</v>
@@ -5333,7 +5277,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:8">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -5359,7 +5303,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:8">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -5385,7 +5329,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:8">
       <c r="A146" s="1">
         <v>144</v>
       </c>
@@ -5411,7 +5355,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:8">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -5437,7 +5381,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:8">
       <c r="A148" s="1">
         <v>146</v>
       </c>
@@ -5463,7 +5407,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:8">
       <c r="A149" s="1">
         <v>147</v>
       </c>
@@ -5489,7 +5433,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:8">
       <c r="A150" s="1">
         <v>148</v>
       </c>
@@ -5515,7 +5459,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:8">
       <c r="A151" s="1">
         <v>149</v>
       </c>
@@ -5541,7 +5485,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:8">
       <c r="A152" s="1">
         <v>150</v>
       </c>
@@ -5567,7 +5511,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:8">
       <c r="A153" s="1">
         <v>151</v>
       </c>
@@ -5593,7 +5537,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:8">
       <c r="A154" s="1">
         <v>152</v>
       </c>
@@ -5619,7 +5563,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:8">
       <c r="A155" s="1">
         <v>153</v>
       </c>
@@ -5645,7 +5589,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:8">
       <c r="A156" s="1">
         <v>154</v>
       </c>
@@ -5653,7 +5597,7 @@
         <v>161</v>
       </c>
       <c r="C156">
-        <v>18.399999999999999</v>
+        <v>18.4</v>
       </c>
       <c r="D156">
         <v>734.5</v>
@@ -5671,7 +5615,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:8">
       <c r="A157" s="1">
         <v>155</v>
       </c>
@@ -5697,7 +5641,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:8">
       <c r="A158" s="1">
         <v>156</v>
       </c>
@@ -5723,7 +5667,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:8">
       <c r="A159" s="1">
         <v>157</v>
       </c>
@@ -5749,7 +5693,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:8">
       <c r="A160" s="1">
         <v>158</v>
       </c>
@@ -5757,7 +5701,7 @@
         <v>165</v>
       </c>
       <c r="C160">
-        <v>19.899999999999999</v>
+        <v>19.9</v>
       </c>
       <c r="D160">
         <v>735.8</v>
@@ -5775,7 +5719,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:8">
       <c r="A161" s="1">
         <v>159</v>
       </c>
@@ -5801,7 +5745,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:8">
       <c r="A162" s="1">
         <v>160</v>
       </c>
@@ -5827,7 +5771,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:8">
       <c r="A163" s="1">
         <v>161</v>
       </c>
@@ -5853,7 +5797,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:8">
       <c r="A164" s="1">
         <v>162</v>
       </c>
@@ -5879,7 +5823,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:8">
       <c r="A165" s="1">
         <v>163</v>
       </c>
@@ -5905,7 +5849,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:8">
       <c r="A166" s="1">
         <v>164</v>
       </c>
@@ -5931,7 +5875,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:8">
       <c r="A167" s="1">
         <v>165</v>
       </c>
@@ -5957,7 +5901,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:8">
       <c r="A168" s="1">
         <v>166</v>
       </c>
@@ -5983,7 +5927,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:8">
       <c r="A169" s="1">
         <v>167</v>
       </c>
@@ -6009,7 +5953,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:8">
       <c r="A170" s="1">
         <v>168</v>
       </c>
@@ -6035,7 +5979,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:8">
       <c r="A171" s="1">
         <v>169</v>
       </c>
@@ -6061,7 +6005,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:8">
       <c r="A172" s="1">
         <v>170</v>
       </c>
@@ -6087,7 +6031,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:8">
       <c r="A173" s="1">
         <v>171</v>
       </c>
@@ -6113,7 +6057,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:8">
       <c r="A174" s="1">
         <v>172</v>
       </c>
@@ -6139,7 +6083,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:8">
       <c r="A175" s="1">
         <v>173</v>
       </c>
@@ -6165,7 +6109,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:8">
       <c r="A176" s="1">
         <v>174</v>
       </c>
@@ -6191,7 +6135,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:8">
       <c r="A177" s="1">
         <v>175</v>
       </c>
@@ -6217,7 +6161,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:8">
       <c r="A178" s="1">
         <v>176</v>
       </c>
@@ -6243,7 +6187,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:8">
       <c r="A179" s="1">
         <v>177</v>
       </c>
@@ -6269,7 +6213,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:8">
       <c r="A180" s="1">
         <v>178</v>
       </c>
@@ -6295,7 +6239,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:8">
       <c r="A181" s="1">
         <v>179</v>
       </c>
@@ -6321,7 +6265,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:8">
       <c r="A182" s="1">
         <v>180</v>
       </c>
@@ -6347,7 +6291,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:8">
       <c r="A183" s="1">
         <v>181</v>
       </c>
@@ -6373,7 +6317,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:8">
       <c r="A184" s="1">
         <v>182</v>
       </c>
@@ -6399,7 +6343,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:8">
       <c r="A185" s="1">
         <v>183</v>
       </c>
@@ -6425,7 +6369,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:8">
       <c r="A186" s="1">
         <v>184</v>
       </c>
@@ -6451,7 +6395,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:8">
       <c r="A187" s="1">
         <v>185</v>
       </c>
@@ -6477,7 +6421,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:8">
       <c r="A188" s="1">
         <v>186</v>
       </c>
@@ -6503,7 +6447,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:8">
       <c r="A189" s="1">
         <v>187</v>
       </c>
@@ -6529,7 +6473,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:8">
       <c r="A190" s="1">
         <v>188</v>
       </c>
@@ -6555,7 +6499,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:8">
       <c r="A191" s="1">
         <v>189</v>
       </c>
@@ -6581,7 +6525,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:8">
       <c r="A192" s="1">
         <v>190</v>
       </c>
@@ -6607,7 +6551,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:8">
       <c r="A193" s="1">
         <v>191</v>
       </c>
@@ -6633,7 +6577,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:8">
       <c r="A194" s="1">
         <v>192</v>
       </c>
@@ -6659,7 +6603,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:8">
       <c r="A195" s="1">
         <v>193</v>
       </c>
@@ -6685,7 +6629,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:8">
       <c r="A196" s="1">
         <v>194</v>
       </c>
@@ -6693,7 +6637,7 @@
         <v>201</v>
       </c>
       <c r="C196">
-        <v>19.399999999999999</v>
+        <v>19.4</v>
       </c>
       <c r="D196">
         <v>735.1</v>
@@ -6711,7 +6655,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:8">
       <c r="A197" s="1">
         <v>195</v>
       </c>
@@ -6737,7 +6681,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:8">
       <c r="A198" s="1">
         <v>196</v>
       </c>
@@ -6763,7 +6707,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:8">
       <c r="A199" s="1">
         <v>197</v>
       </c>
@@ -6789,7 +6733,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:8">
       <c r="A200" s="1">
         <v>198</v>
       </c>
@@ -6815,7 +6759,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:8">
       <c r="A201" s="1">
         <v>199</v>
       </c>
@@ -6841,7 +6785,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:8">
       <c r="A202" s="1">
         <v>200</v>
       </c>
@@ -6867,7 +6811,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:8">
       <c r="A203" s="1">
         <v>201</v>
       </c>
@@ -6893,7 +6837,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:8">
       <c r="A204" s="1">
         <v>202</v>
       </c>
@@ -6919,7 +6863,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:8">
       <c r="A205" s="1">
         <v>203</v>
       </c>
@@ -6945,7 +6889,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:8">
       <c r="A206" s="1">
         <v>204</v>
       </c>
@@ -6971,7 +6915,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:8">
       <c r="A207" s="1">
         <v>205</v>
       </c>
@@ -6979,7 +6923,7 @@
         <v>212</v>
       </c>
       <c r="C207">
-        <v>8.1999999999999993</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="D207">
         <v>734.2</v>
@@ -6997,7 +6941,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:8">
       <c r="A208" s="1">
         <v>206</v>
       </c>
@@ -7023,7 +6967,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:8">
       <c r="A209" s="1">
         <v>207</v>
       </c>
@@ -7049,7 +6993,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:8">
       <c r="A210" s="1">
         <v>208</v>
       </c>
@@ -7075,7 +7019,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:8">
       <c r="A211" s="1">
         <v>209</v>
       </c>
@@ -7101,7 +7045,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:8">
       <c r="A212" s="1">
         <v>210</v>
       </c>
@@ -7109,7 +7053,7 @@
         <v>217</v>
       </c>
       <c r="C212">
-        <v>17.100000000000001</v>
+        <v>17.1</v>
       </c>
       <c r="D212">
         <v>732.1</v>
@@ -7127,7 +7071,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:8">
       <c r="A213" s="1">
         <v>211</v>
       </c>
@@ -7153,7 +7097,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:8">
       <c r="A214" s="1">
         <v>212</v>
       </c>
@@ -7161,7 +7105,7 @@
         <v>219</v>
       </c>
       <c r="C214">
-        <v>5.0999999999999996</v>
+        <v>5.1</v>
       </c>
       <c r="D214">
         <v>730.3</v>
@@ -7179,7 +7123,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:8">
       <c r="A215" s="1">
         <v>213</v>
       </c>
@@ -7187,7 +7131,7 @@
         <v>220</v>
       </c>
       <c r="C215">
-        <v>4.5999999999999996</v>
+        <v>4.6</v>
       </c>
       <c r="D215">
         <v>731</v>
@@ -7205,7 +7149,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:8">
       <c r="A216" s="1">
         <v>214</v>
       </c>
@@ -7231,7 +7175,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:8">
       <c r="A217" s="1">
         <v>215</v>
       </c>
@@ -7257,7 +7201,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:8">
       <c r="A218" s="1">
         <v>216</v>
       </c>
@@ -7283,7 +7227,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:8">
       <c r="A219" s="1">
         <v>217</v>
       </c>
@@ -7309,7 +7253,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:8">
       <c r="A220" s="1">
         <v>218</v>
       </c>
@@ -7335,7 +7279,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:8">
       <c r="A221" s="1">
         <v>219</v>
       </c>
@@ -7361,7 +7305,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:8">
       <c r="A222" s="1">
         <v>220</v>
       </c>
@@ -7387,7 +7331,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:8">
       <c r="A223" s="1">
         <v>221</v>
       </c>
@@ -7413,7 +7357,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:8">
       <c r="A224" s="1">
         <v>222</v>
       </c>
@@ -7439,7 +7383,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:8">
       <c r="A225" s="1">
         <v>223</v>
       </c>
@@ -7465,7 +7409,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:8">
       <c r="A226" s="1">
         <v>224</v>
       </c>
@@ -7491,7 +7435,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:8">
       <c r="A227" s="1">
         <v>225</v>
       </c>
@@ -7517,7 +7461,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:8">
       <c r="A228" s="1">
         <v>226</v>
       </c>
@@ -7543,7 +7487,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:8">
       <c r="A229" s="1">
         <v>227</v>
       </c>
@@ -7569,7 +7513,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:8">
       <c r="A230" s="1">
         <v>228</v>
       </c>
@@ -7595,7 +7539,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:8">
       <c r="A231" s="1">
         <v>229</v>
       </c>
@@ -7621,7 +7565,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:8">
       <c r="A232" s="1">
         <v>230</v>
       </c>
@@ -7647,7 +7591,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:8">
       <c r="A233" s="1">
         <v>231</v>
       </c>
@@ -7673,7 +7617,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:8">
       <c r="A234" s="1">
         <v>232</v>
       </c>
@@ -7699,7 +7643,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:8">
       <c r="A235" s="1">
         <v>233</v>
       </c>
@@ -7725,7 +7669,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:8">
       <c r="A236" s="1">
         <v>234</v>
       </c>
@@ -7751,7 +7695,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="237" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:8">
       <c r="A237" s="1">
         <v>235</v>
       </c>
@@ -7777,7 +7721,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:8">
       <c r="A238" s="1">
         <v>236</v>
       </c>
@@ -7803,7 +7747,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:8">
       <c r="A239" s="1">
         <v>237</v>
       </c>
@@ -7811,7 +7755,7 @@
         <v>244</v>
       </c>
       <c r="C239">
-        <v>9.1999999999999993</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="D239">
         <v>741.2</v>
@@ -7829,7 +7773,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:8">
       <c r="A240" s="1">
         <v>238</v>
       </c>
@@ -7855,7 +7799,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:8">
       <c r="A241" s="1">
         <v>239</v>
       </c>
@@ -7881,7 +7825,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:8">
       <c r="A242" s="1">
         <v>240</v>
       </c>
@@ -7907,7 +7851,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="243" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:8">
       <c r="A243" s="1">
         <v>241</v>
       </c>
@@ -7933,7 +7877,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:8">
       <c r="A244" s="1">
         <v>242</v>
       </c>
@@ -7959,7 +7903,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:8">
       <c r="A245" s="1">
         <v>243</v>
       </c>
@@ -7985,7 +7929,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="246" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:8">
       <c r="A246" s="1">
         <v>244</v>
       </c>
@@ -8011,7 +7955,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="247" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:8">
       <c r="A247" s="1">
         <v>245</v>
       </c>
@@ -8037,7 +7981,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:8">
       <c r="A248" s="1">
         <v>246</v>
       </c>
@@ -8063,7 +8007,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="249" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:8">
       <c r="A249" s="1">
         <v>247</v>
       </c>
@@ -8089,7 +8033,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="250" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:8">
       <c r="A250" s="1">
         <v>248</v>
       </c>
@@ -8097,7 +8041,7 @@
         <v>255</v>
       </c>
       <c r="C250">
-        <v>8.3000000000000007</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="D250">
         <v>737.4</v>
@@ -8115,7 +8059,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="251" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:8">
       <c r="A251" s="1">
         <v>249</v>
       </c>
@@ -8141,7 +8085,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="252" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:8">
       <c r="A252" s="1">
         <v>250</v>
       </c>
@@ -8167,7 +8111,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="253" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:8">
       <c r="A253" s="1">
         <v>251</v>
       </c>
@@ -8193,7 +8137,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="254" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:8">
       <c r="A254" s="1">
         <v>252</v>
       </c>
@@ -8219,7 +8163,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="255" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:8">
       <c r="A255" s="1">
         <v>253</v>
       </c>
@@ -8227,7 +8171,7 @@
         <v>260</v>
       </c>
       <c r="C255">
-        <v>2.2999999999999998</v>
+        <v>2.3</v>
       </c>
       <c r="D255">
         <v>730.5</v>
@@ -8245,7 +8189,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="256" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:8">
       <c r="A256" s="1">
         <v>254</v>
       </c>
@@ -8271,7 +8215,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="257" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:8">
       <c r="A257" s="1">
         <v>255</v>
       </c>
@@ -8297,7 +8241,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="258" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:8">
       <c r="A258" s="1">
         <v>256</v>
       </c>
@@ -8305,7 +8249,7 @@
         <v>263</v>
       </c>
       <c r="C258">
-        <v>9.3000000000000007</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="D258">
         <v>733.8</v>
@@ -8323,7 +8267,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="259" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:8">
       <c r="A259" s="1">
         <v>257</v>
       </c>
@@ -8349,7 +8293,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="260" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:8">
       <c r="A260" s="1">
         <v>258</v>
       </c>
@@ -8375,7 +8319,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="261" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:8">
       <c r="A261" s="1">
         <v>259</v>
       </c>
@@ -8401,7 +8345,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="262" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:8">
       <c r="A262" s="1">
         <v>260</v>
       </c>
@@ -8427,7 +8371,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="263" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:8">
       <c r="A263" s="1">
         <v>261</v>
       </c>
@@ -8435,7 +8379,7 @@
         <v>268</v>
       </c>
       <c r="C263">
-        <v>4.0999999999999996</v>
+        <v>4.1</v>
       </c>
       <c r="D263">
         <v>737.4</v>
@@ -8453,7 +8397,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="264" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:8">
       <c r="A264" s="1">
         <v>262</v>
       </c>
@@ -8479,7 +8423,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="265" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:8">
       <c r="A265" s="1">
         <v>263</v>
       </c>
@@ -8505,7 +8449,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="266" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:8">
       <c r="A266" s="1">
         <v>264</v>
       </c>
@@ -8531,7 +8475,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="267" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:8">
       <c r="A267" s="1">
         <v>265</v>
       </c>
@@ -8557,7 +8501,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="268" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:8">
       <c r="A268" s="1">
         <v>266</v>
       </c>
@@ -8583,7 +8527,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="269" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:8">
       <c r="A269" s="1">
         <v>267</v>
       </c>
@@ -8609,7 +8553,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="270" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:8">
       <c r="A270" s="1">
         <v>268</v>
       </c>
@@ -8617,7 +8561,7 @@
         <v>275</v>
       </c>
       <c r="C270">
-        <v>-4.9000000000000004</v>
+        <v>-4.9</v>
       </c>
       <c r="D270">
         <v>743.9</v>
@@ -8635,7 +8579,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="271" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:8">
       <c r="A271" s="1">
         <v>269</v>
       </c>
@@ -8661,7 +8605,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="272" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:8">
       <c r="A272" s="1">
         <v>270</v>
       </c>
@@ -8687,7 +8631,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="273" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:8">
       <c r="A273" s="1">
         <v>271</v>
       </c>
@@ -8713,7 +8657,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="274" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:8">
       <c r="A274" s="1">
         <v>272</v>
       </c>
@@ -8739,7 +8683,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:8">
       <c r="A275" s="1">
         <v>273</v>
       </c>
@@ -8765,7 +8709,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:8">
       <c r="A276" s="1">
         <v>274</v>
       </c>
@@ -8791,7 +8735,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:8">
       <c r="A277" s="1">
         <v>275</v>
       </c>
@@ -8817,7 +8761,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="278" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:8">
       <c r="A278" s="1">
         <v>276</v>
       </c>
@@ -8843,7 +8787,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="279" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:8">
       <c r="A279" s="1">
         <v>277</v>
       </c>
@@ -8869,7 +8813,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="280" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:8">
       <c r="A280" s="1">
         <v>278</v>
       </c>
@@ -8895,7 +8839,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="281" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:8">
       <c r="A281" s="1">
         <v>279</v>
       </c>
@@ -8921,7 +8865,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="282" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:8">
       <c r="A282" s="1">
         <v>280</v>
       </c>
@@ -8947,7 +8891,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="283" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:8">
       <c r="A283" s="1">
         <v>281</v>
       </c>
@@ -8973,7 +8917,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="284" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:8">
       <c r="A284" s="1">
         <v>282</v>
       </c>
@@ -8999,7 +8943,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="285" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:8">
       <c r="A285" s="1">
         <v>283</v>
       </c>
@@ -9025,7 +8969,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="286" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:8">
       <c r="A286" s="1">
         <v>284</v>
       </c>
@@ -9033,7 +8977,7 @@
         <v>291</v>
       </c>
       <c r="C286">
-        <v>-5.0999999999999996</v>
+        <v>-5.1</v>
       </c>
       <c r="D286">
         <v>742.9</v>
@@ -9051,7 +8995,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="287" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:8">
       <c r="A287" s="1">
         <v>285</v>
       </c>
@@ -9077,7 +9021,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="288" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:8">
       <c r="A288" s="1">
         <v>286</v>
       </c>
@@ -9103,7 +9047,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="289" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:8">
       <c r="A289" s="1">
         <v>287</v>
       </c>
@@ -9111,7 +9055,7 @@
         <v>294</v>
       </c>
       <c r="C289">
-        <v>-9.8000000000000007</v>
+        <v>-9.800000000000001</v>
       </c>
       <c r="D289">
         <v>745.6</v>
@@ -9129,7 +9073,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="290" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:8">
       <c r="A290" s="1">
         <v>288</v>
       </c>
@@ -9155,7 +9099,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="291" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:8">
       <c r="A291" s="1">
         <v>289</v>
       </c>
@@ -9181,7 +9125,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="292" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:8">
       <c r="A292" s="1">
         <v>290</v>
       </c>
@@ -9207,7 +9151,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="293" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:8">
       <c r="A293" s="1">
         <v>291</v>
       </c>
@@ -9233,7 +9177,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="294" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:8">
       <c r="A294" s="1">
         <v>292</v>
       </c>
@@ -9259,7 +9203,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="295" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:8">
       <c r="A295" s="1">
         <v>293</v>
       </c>
@@ -9285,7 +9229,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="296" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:8">
       <c r="A296" s="1">
         <v>294</v>
       </c>
@@ -9311,7 +9255,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="297" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:8">
       <c r="A297" s="1">
         <v>295</v>
       </c>
@@ -9337,7 +9281,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="298" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:8">
       <c r="A298" s="1">
         <v>296</v>
       </c>
@@ -9363,7 +9307,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="299" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:8">
       <c r="A299" s="1">
         <v>297</v>
       </c>
@@ -9389,7 +9333,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="300" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:8">
       <c r="A300" s="1">
         <v>298</v>
       </c>
@@ -9415,7 +9359,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="301" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:8">
       <c r="A301" s="1">
         <v>299</v>
       </c>
@@ -9441,7 +9385,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="302" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:8">
       <c r="A302" s="1">
         <v>300</v>
       </c>
@@ -9467,7 +9411,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="303" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:8">
       <c r="A303" s="1">
         <v>301</v>
       </c>
@@ -9493,7 +9437,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="304" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:8">
       <c r="A304" s="1">
         <v>302</v>
       </c>
@@ -9519,7 +9463,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="305" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:8">
       <c r="A305" s="1">
         <v>303</v>
       </c>
@@ -9545,7 +9489,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="306" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:8">
       <c r="A306" s="1">
         <v>304</v>
       </c>
@@ -9571,7 +9515,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="307" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:8">
       <c r="A307" s="1">
         <v>305</v>
       </c>
@@ -9597,7 +9541,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="308" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:8">
       <c r="A308" s="1">
         <v>306</v>
       </c>
@@ -9623,7 +9567,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="309" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:8">
       <c r="A309" s="1">
         <v>307</v>
       </c>
@@ -9649,7 +9593,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="310" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:8">
       <c r="A310" s="1">
         <v>308</v>
       </c>
@@ -9675,7 +9619,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="311" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:8">
       <c r="A311" s="1">
         <v>309</v>
       </c>
@@ -9701,7 +9645,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="312" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:8">
       <c r="A312" s="1">
         <v>310</v>
       </c>
@@ -9727,7 +9671,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="313" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:8">
       <c r="A313" s="1">
         <v>311</v>
       </c>
@@ -9753,7 +9697,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="314" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:8">
       <c r="A314" s="1">
         <v>312</v>
       </c>
@@ -9779,7 +9723,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="315" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:8">
       <c r="A315" s="1">
         <v>313</v>
       </c>
@@ -9805,7 +9749,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="316" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:8">
       <c r="A316" s="1">
         <v>314</v>
       </c>
@@ -9831,7 +9775,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="317" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:8">
       <c r="A317" s="1">
         <v>315</v>
       </c>
@@ -9857,7 +9801,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="318" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:8">
       <c r="A318" s="1">
         <v>316</v>
       </c>
@@ -9883,7 +9827,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="319" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:8">
       <c r="A319" s="1">
         <v>317</v>
       </c>
@@ -9891,7 +9835,7 @@
         <v>324</v>
       </c>
       <c r="C319">
-        <v>-8.1999999999999993</v>
+        <v>-8.199999999999999</v>
       </c>
       <c r="D319">
         <v>759.3</v>
@@ -9909,7 +9853,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="320" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:8">
       <c r="A320" s="1">
         <v>318</v>
       </c>
@@ -9935,7 +9879,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="321" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:8">
       <c r="A321" s="1">
         <v>319</v>
       </c>
@@ -9961,7 +9905,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="322" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:8">
       <c r="A322" s="1">
         <v>320</v>
       </c>
@@ -9987,7 +9931,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="323" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:8">
       <c r="A323" s="1">
         <v>321</v>
       </c>
@@ -10013,7 +9957,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="324" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:8">
       <c r="A324" s="1">
         <v>322</v>
       </c>
@@ -10039,7 +9983,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="325" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:8">
       <c r="A325" s="1">
         <v>323</v>
       </c>
@@ -10065,7 +10009,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="326" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:8">
       <c r="A326" s="1">
         <v>324</v>
       </c>
@@ -10091,7 +10035,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="327" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:8">
       <c r="A327" s="1">
         <v>325</v>
       </c>
@@ -10117,7 +10061,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="328" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:8">
       <c r="A328" s="1">
         <v>326</v>
       </c>
@@ -10125,7 +10069,7 @@
         <v>333</v>
       </c>
       <c r="C328">
-        <v>-16.600000000000001</v>
+        <v>-16.6</v>
       </c>
       <c r="D328">
         <v>752.1</v>
@@ -10143,7 +10087,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="329" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:8">
       <c r="A329" s="1">
         <v>327</v>
       </c>
@@ -10169,7 +10113,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="330" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:8">
       <c r="A330" s="1">
         <v>328</v>
       </c>
@@ -10195,7 +10139,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="331" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:8">
       <c r="A331" s="1">
         <v>329</v>
       </c>
@@ -10221,7 +10165,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="332" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:8">
       <c r="A332" s="1">
         <v>330</v>
       </c>
@@ -10247,7 +10191,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="333" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:8">
       <c r="A333" s="1">
         <v>331</v>
       </c>
@@ -10273,7 +10217,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="334" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:8">
       <c r="A334" s="1">
         <v>332</v>
       </c>
@@ -10299,7 +10243,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="335" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:8">
       <c r="A335" s="1">
         <v>333</v>
       </c>
@@ -10325,7 +10269,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="336" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:8">
       <c r="A336" s="1">
         <v>334</v>
       </c>
@@ -10351,7 +10295,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="337" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:8">
       <c r="A337" s="1">
         <v>335</v>
       </c>
@@ -10377,7 +10321,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="338" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:8">
       <c r="A338" s="1">
         <v>336</v>
       </c>
@@ -10403,7 +10347,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="339" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:8">
       <c r="A339" s="1">
         <v>337</v>
       </c>
@@ -10429,7 +10373,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="340" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:8">
       <c r="A340" s="1">
         <v>338</v>
       </c>
@@ -10455,7 +10399,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="341" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:8">
       <c r="A341" s="1">
         <v>339</v>
       </c>
@@ -10463,7 +10407,7 @@
         <v>346</v>
       </c>
       <c r="C341">
-        <v>-8.6999999999999993</v>
+        <v>-8.699999999999999</v>
       </c>
       <c r="D341">
         <v>736.6</v>
@@ -10481,7 +10425,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="342" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:8">
       <c r="A342" s="1">
         <v>340</v>
       </c>
@@ -10507,7 +10451,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="343" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:8">
       <c r="A343" s="1">
         <v>341</v>
       </c>
@@ -10533,7 +10477,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="344" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:8">
       <c r="A344" s="1">
         <v>342</v>
       </c>
@@ -10559,7 +10503,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="345" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:8">
       <c r="A345" s="1">
         <v>343</v>
       </c>
@@ -10585,7 +10529,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="346" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:8">
       <c r="A346" s="1">
         <v>344</v>
       </c>
@@ -10611,7 +10555,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="347" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:8">
       <c r="A347" s="1">
         <v>345</v>
       </c>
@@ -10637,7 +10581,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="348" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:8">
       <c r="A348" s="1">
         <v>346</v>
       </c>
@@ -10663,7 +10607,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="349" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:8">
       <c r="A349" s="1">
         <v>347</v>
       </c>
@@ -10689,7 +10633,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="350" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:8">
       <c r="A350" s="1">
         <v>348</v>
       </c>
@@ -10697,7 +10641,7 @@
         <v>355</v>
       </c>
       <c r="C350">
-        <v>-16.100000000000001</v>
+        <v>-16.1</v>
       </c>
       <c r="D350">
         <v>752.4</v>
@@ -10715,7 +10659,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="351" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:8">
       <c r="A351" s="1">
         <v>349</v>
       </c>
@@ -10741,7 +10685,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="352" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:8">
       <c r="A352" s="1">
         <v>350</v>
       </c>
@@ -10749,7 +10693,7 @@
         <v>357</v>
       </c>
       <c r="C352">
-        <v>-18.600000000000001</v>
+        <v>-18.6</v>
       </c>
       <c r="D352">
         <v>753.1</v>
@@ -10767,7 +10711,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="353" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:8">
       <c r="A353" s="1">
         <v>351</v>
       </c>
@@ -10793,7 +10737,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="354" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:8">
       <c r="A354" s="1">
         <v>352</v>
       </c>
@@ -10819,7 +10763,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="355" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:8">
       <c r="A355" s="1">
         <v>353</v>
       </c>
@@ -10845,7 +10789,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="356" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:8">
       <c r="A356" s="1">
         <v>354</v>
       </c>
@@ -10871,7 +10815,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="357" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:8">
       <c r="A357" s="1">
         <v>355</v>
       </c>

</xml_diff>